<commit_message>
Lorte ramasjang lort TRP
</commit_message>
<xml_diff>
--- a/data/data_inventory_consumption.xlsx
+++ b/data/data_inventory_consumption.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3669516081e98610/Dokumenter/Uni/Speciale/Git/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{2AC5AAAA-F157-AA49-9BBB-8EF8A2ACBC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF8B1669-7221-4FBB-BC25-62D81DD2AA0E}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{2AC5AAAA-F157-AA49-9BBB-8EF8A2ACBC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8E38C89-9E94-4315-938A-FBC9B3A5FCFF}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="2160" windowWidth="25440" windowHeight="15270" firstSheet="23" activeTab="31" xr2:uid="{4ABCB470-47AD-4A8F-A8F9-A418E061C63E}"/>
+    <workbookView xWindow="43080" yWindow="2160" windowWidth="25440" windowHeight="15270" firstSheet="16" activeTab="21" xr2:uid="{4ABCB470-47AD-4A8F-A8F9-A418E061C63E}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="41">
   <si>
     <t>DR1</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>DR Radio</t>
+  </si>
+  <si>
+    <t>* Ændret pga Ramasjang TRP</t>
   </si>
 </sst>
 </file>
@@ -7218,15 +7221,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F53B346-D6CA-9D4C-86C0-CCD3D74D1B59}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -7261,7 +7264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -7270,16 +7273,20 @@
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>100</v>
+        <f>50.7/4</f>
+        <v>12.675000000000001</v>
       </c>
       <c r="E2" s="2">
-        <v>100</v>
+        <f t="shared" ref="E2:G2" si="0">50.7/4</f>
+        <v>12.675000000000001</v>
       </c>
       <c r="F2" s="2">
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>12.675000000000001</v>
       </c>
       <c r="G2" s="2">
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>12.675000000000001</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -7292,7 +7299,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -7323,7 +7330,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -7335,38 +7342,41 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:J4" si="0">D2*$K4/100</f>
+        <f t="shared" ref="D4:J4" si="1">D2*$K4/100</f>
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2</v>
       </c>
@@ -7378,38 +7388,38 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:J5" si="1">D2*$K5/100</f>
+        <f t="shared" ref="D5:J5" si="2">D2*$K5/100</f>
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
@@ -7421,38 +7431,38 @@
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D6:J6" si="2">D2*$K6/100</f>
-        <v>100</v>
+        <f>D2*$K6/100</f>
+        <v>12.675000000000001</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f t="shared" ref="E6:G6" si="3">E2*$K6/100</f>
+        <v>12.675000000000001</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f t="shared" si="3"/>
+        <v>12.675000000000001</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f t="shared" si="3"/>
+        <v>12.675000000000001</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D6:J6" si="4">H2*$K6/100</f>
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K6" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4</v>
       </c>
@@ -7464,38 +7474,38 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:J8" si="3">D$3*$K7/100</f>
+        <f t="shared" ref="D7:J8" si="5">D$3*$K7/100</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5</v>
       </c>
@@ -7507,38 +7517,38 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>6</v>
       </c>
@@ -7546,42 +7556,42 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:J13" si="4">C$3*$K9/100</f>
+        <f t="shared" ref="C9:J13" si="6">C$3*$K9/100</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>7</v>
       </c>
@@ -7589,42 +7599,42 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>8</v>
       </c>
@@ -7632,42 +7642,42 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9</v>
       </c>
@@ -7675,42 +7685,42 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10</v>
       </c>
@@ -7718,42 +7728,42 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>11</v>
       </c>
@@ -7786,7 +7796,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>12</v>
       </c>
@@ -7829,15 +7839,15 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0900FE42-DEF3-AD4D-8233-E77D6BFF956F}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -7872,7 +7882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -7884,13 +7894,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>60</v>
+        <f>21/3</f>
+        <v>7</v>
       </c>
       <c r="F2" s="2">
-        <v>60</v>
+        <f t="shared" ref="F2:G2" si="0">21/3</f>
+        <v>7</v>
       </c>
       <c r="G2" s="2">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -7903,7 +7916,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -7934,7 +7947,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -7946,38 +7959,41 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:J4" si="0">D2*$K4/100</f>
+        <f t="shared" ref="D4:J4" si="1">D2*$K4/100</f>
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2</v>
       </c>
@@ -7989,38 +8005,38 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:J5" si="1">D2*$K5/100</f>
+        <f t="shared" ref="D5:J5" si="2">D2*$K5/100</f>
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
@@ -8032,38 +8048,38 @@
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D6:J6" si="2">D2*$K6/100</f>
+        <f t="shared" ref="D6:J6" si="3">D2*$K6/100</f>
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K6" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4</v>
       </c>
@@ -8075,38 +8091,38 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:J8" si="3">D$3*$K7/100</f>
+        <f t="shared" ref="D7:J8" si="4">D$3*$K7/100</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5</v>
       </c>
@@ -8118,38 +8134,38 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>6</v>
       </c>
@@ -8157,42 +8173,42 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:J13" si="4">C$3*$K9/100</f>
+        <f t="shared" ref="C9:J13" si="5">C$3*$K9/100</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>7</v>
       </c>
@@ -8200,42 +8216,42 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>8</v>
       </c>
@@ -8243,42 +8259,42 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9</v>
       </c>
@@ -8286,42 +8302,42 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10</v>
       </c>
@@ -8329,42 +8345,42 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>11</v>
       </c>
@@ -8397,7 +8413,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>12</v>
       </c>
@@ -8440,15 +8456,15 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320E5E6B-3822-3D48-AD5A-C084835E6C97}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -8483,7 +8499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -8514,7 +8530,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -8544,8 +8560,10 @@
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -8553,42 +8571,45 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <f>C2*$K4/100</f>
-        <v>18.7</v>
+        <f>54*C2/450</f>
+        <v>20.399999999999999</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:J4" si="0">D2*$K4/100</f>
-        <v>18.7</v>
+        <f t="shared" ref="D4:E4" si="0">54*D2/450</f>
+        <v>20.399999999999999</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>12.1</v>
+        <v>13.2</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D4:J4" si="1">F2*$K4/100</f>
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2</v>
       </c>
@@ -8600,38 +8621,38 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:J5" si="1">D2*$K5/100</f>
+        <f t="shared" ref="D5:J5" si="2">D2*$K5/100</f>
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
@@ -8639,42 +8660,42 @@
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <f>C2*$K6/100</f>
-        <v>151.30000000000001</v>
+        <f>66*C2/450</f>
+        <v>24.933333333333334</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D6:J6" si="2">D2*$K6/100</f>
-        <v>151.30000000000001</v>
+        <f t="shared" ref="D6:E6" si="3">66*D2/450</f>
+        <v>24.933333333333334</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="2"/>
-        <v>97.9</v>
+        <f t="shared" si="3"/>
+        <v>16.133333333333333</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D6:J6" si="4">F2*$K6/100</f>
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4</v>
       </c>
@@ -8686,38 +8707,38 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:J8" si="3">D$3*$K7/100</f>
+        <f t="shared" ref="D7:J8" si="5">D$3*$K7/100</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5</v>
       </c>
@@ -8729,38 +8750,38 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>6</v>
       </c>
@@ -8768,42 +8789,42 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:J13" si="4">C$3*$K9/100</f>
+        <f t="shared" ref="C9:J13" si="6">C$3*$K9/100</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>7</v>
       </c>
@@ -8811,42 +8832,42 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>8</v>
       </c>
@@ -8854,42 +8875,42 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9</v>
       </c>
@@ -8897,42 +8918,42 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10</v>
       </c>
@@ -8940,42 +8961,42 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>11</v>
       </c>
@@ -9008,7 +9029,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>12</v>
       </c>
@@ -9051,15 +9072,15 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6FD59A-06A5-DE48-9C20-BF9F17ADA0DB}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -9094,7 +9115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -9106,13 +9127,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -9125,7 +9146,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -9156,7 +9177,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -9172,16 +9193,16 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>4.9000000000000004</v>
+        <f>36/3</f>
+        <v>12</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>4.9000000000000004</v>
+        <f t="shared" ref="F4:G4" si="1">36/3</f>
+        <v>12</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
-        <v>4.9000000000000004</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
@@ -9196,10 +9217,13 @@
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2</v>
       </c>
@@ -9211,38 +9235,38 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:J5" si="1">D2*$K5/100</f>
+        <f t="shared" ref="D5:J5" si="2">D2*$K5/100</f>
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
@@ -9254,38 +9278,38 @@
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D6:J6" si="2">D2*$K6/100</f>
+        <f t="shared" ref="D6:J6" si="3">D2*$K6/100</f>
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="2"/>
-        <v>93.1</v>
+        <f>44/3</f>
+        <v>14.666666666666666</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="2"/>
-        <v>93.1</v>
+        <f t="shared" ref="F6:G6" si="4">44/3</f>
+        <v>14.666666666666666</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="2"/>
-        <v>93.1</v>
+        <f t="shared" si="4"/>
+        <v>14.666666666666666</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4</v>
       </c>
@@ -9297,38 +9321,38 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:J8" si="3">D$3*$K7/100</f>
+        <f t="shared" ref="D7:J8" si="5">D$3*$K7/100</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5</v>
       </c>
@@ -9340,38 +9364,38 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>6</v>
       </c>
@@ -9379,42 +9403,42 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:J13" si="4">C$3*$K9/100</f>
+        <f t="shared" ref="C9:J13" si="6">C$3*$K9/100</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>7</v>
       </c>
@@ -9422,42 +9446,42 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>8</v>
       </c>
@@ -9465,42 +9489,42 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9</v>
       </c>
@@ -9508,42 +9532,42 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10</v>
       </c>
@@ -9551,42 +9575,42 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>11</v>
       </c>
@@ -9619,7 +9643,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>12</v>
       </c>
@@ -15165,7 +15189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AA1E49-D152-4965-A7B7-E3C0F1662842}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>